<commit_message>
add support for @server.arg("*args*)
</commit_message>
<xml_diff>
--- a/xlwingsjs/tests/udf_tests_officejs.xlsx
+++ b/xlwingsjs/tests/udf_tests_officejs.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/xlwingsjs/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/dev/xlwings/xlwingsjs/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3729C6-3182-144A-921D-428C1E5A9B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB61C120-ACDD-C44C-BB7D-B2A9432C88F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4020" yWindow="-21100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1860" yWindow="-21100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -133,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="125">
   <si>
     <t>epected</t>
   </si>
@@ -465,9 +462,6 @@
     <t>read_series_header_noindex</t>
   </si>
   <si>
-    <t>TO RUN THE TESTS: in devserver.py, import udf_test_officejs as custom_functions, then hit Ctrl-Alt-F9</t>
-  </si>
-  <si>
     <t>one</t>
   </si>
   <si>
@@ -505,6 +499,12 @@
   </si>
   <si>
     <t>volatile</t>
+  </si>
+  <si>
+    <t>TO RUN THE TESTS: in devserver.py, uncomment from tests import udf_tests_officejs as custom_functions, then hit Ctrl-Alt-F9</t>
+  </si>
+  <si>
+    <t>varargs_arg_decorator</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -559,6 +559,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -599,7 +606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -651,8 +658,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,111 +697,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="_xldudf_XLWINGS_DEFAULT_ARGS"/>
-      <definedName name="_xldudf_XLWINGS_METHOD_SIGNATURE_WITH_LESS_THAN_1024_CHARACTERS"/>
-      <definedName name="_xldudf_XLWINGS_METHOD_SIGNATURE_WITH_MORE_THAN_1024_CHARACTERS"/>
-      <definedName name="_xldudf_XLWINGS_OPTIONAL_ARGS"/>
-      <definedName name="_xldudf_XLWINGS_READ_2DLIST"/>
-      <definedName name="_xldudf_XLWINGS_READ_DATE"/>
-      <definedName name="_xldudf_XLWINGS_READ_DATE_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_READ_DATES_AS_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_READ_DATES_AS1"/>
-      <definedName name="_xldudf_XLWINGS_READ_DATES_AS2"/>
-      <definedName name="_xldudf_XLWINGS_READ_DATES_AS3"/>
-      <definedName name="_xldudf_XLWINGS_READ_DATETIME"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_0HEADER_0INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_0HEADER_1INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_0HEADER_2INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_1HEADER_0INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_1HEADER_1NAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_1HEADER_1UNNAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_1HEADER_2NAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_2HEADER_0INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_2HEADER_1NAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_2HEADER_1UNNAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_2HEADER_2NAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_2HEADER_2UNNAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DF_DATE_INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_DICT"/>
-      <definedName name="_xldudf_XLWINGS_READ_DICT_TRANSPOSE"/>
-      <definedName name="_xldudf_XLWINGS_READ_EMPTY"/>
-      <definedName name="_xldudf_XLWINGS_READ_EMPTY_AS"/>
-      <definedName name="_xldudf_XLWINGS_READ_EMPTY_AS_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_READ_EMPTY_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_READ_FLOAT"/>
-      <definedName name="_xldudf_XLWINGS_READ_HORIZONTAL_LIST"/>
-      <definedName name="_xldudf_XLWINGS_READ_HORIZONTAL_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_READ_NDIM1"/>
-      <definedName name="_xldudf_XLWINGS_READ_NDIM1_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_READ_NDIM2"/>
-      <definedName name="_xldudf_XLWINGS_READ_NDIM2_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_READ_SCALAR_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_READ_SERIES_HEADER_NAMED_2INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_SERIES_HEADER_NAMED_INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_SERIES_HEADER_NAMELESS_2INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_SERIES_HEADER_NAMELESS_INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_SERIES_HEADER_NOINDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_SERIES_NOHEADER_2INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_SERIES_NOHEADER_INDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_SERIES_NOHEADER_NOINDEX"/>
-      <definedName name="_xldudf_XLWINGS_READ_STRING"/>
-      <definedName name="_xldudf_XLWINGS_READ_TIMESERIES"/>
-      <definedName name="_xldudf_XLWINGS_READ_TRANSPOSE"/>
-      <definedName name="_xldudf_XLWINGS_READ_TRANSPOSE_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_READ_VERTICAL_LIST"/>
-      <definedName name="_xldudf_XLWINGS_READ_VERTICAL_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_RETURN_PD_NAT"/>
-      <definedName name="_xldudf_XLWINGS_VARIABLE_ARGS"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_2DLIST"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DATE"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DATETIME"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_0HEADER_0INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_0HEADER_1INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_0HEADER_2INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_1HEADER_0INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_1HEADER_1NAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_1HEADER_1UNNAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_1HEADER_2NAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_2HEADER_0INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_2HEADER_1NAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_2HEADER_1UNNAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_2HEADER_2NAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_2HEADER_2UNNAMEDINDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DF_DATE_INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_DICT"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_FLOAT"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_HORIZONTAL_LIST"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_NONE"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_NP_SCALAR"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMED_2INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMED_INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMELESS_2INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMELESS_INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_SERIES_HEADER_NOINDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_SERIES_NAN"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_SERIES_NOHEADER_2INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_SERIES_NOHEADER_INDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_SERIES_NOHEADER_NOINDEX"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_STRING"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_TIMESERIES"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_TRANSPOSE"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_TRANSPOSE_NPARRAY"/>
-      <definedName name="_xldudf_XLWINGS_WRITE_VERTICAL_LIST"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1258,103 +1159,110 @@
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
-      <we:containsCustomFunctions/>
+      <we:containsCustomFunctions val="1"/>
     </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
-        <we:customFunctionIds>_xldudf_XLWINGS_ADD</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_ADD2</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_DEFAULT_ARGS</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_METHOD_SIGNATURE_WITH_LESS_THAN_1024_CHARACTERS</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_METHOD_SIGNATURE_WITH_MORE_THAN_1024_CHARACTERS</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_OPTIONAL_ARGS</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_2DLIST</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DATE</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DATE_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DATES_AS1</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DATES_AS2</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DATES_AS3</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DATES_AS_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DATETIME</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_0HEADER_0INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_0HEADER_1INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_0HEADER_2INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_1HEADER_0INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_1HEADER_1NAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_1HEADER_1UNNAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_1HEADER_2NAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_2HEADER_0INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_2HEADER_1NAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_2HEADER_1UNNAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_2HEADER_2NAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_2HEADER_2UNNAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DF_DATE_INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DICT</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_DICT_TRANSPOSE</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_EMPTY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_EMPTY_AS</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_EMPTY_AS_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_EMPTY_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_FLOAT</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_HORIZONTAL_LIST</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_HORIZONTAL_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_NDIM1</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_NDIM1_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_NDIM2</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_NDIM2_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_SCALAR_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_SERIES_HEADER_NAMED_2INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_SERIES_HEADER_NAMED_INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_SERIES_HEADER_NAMELESS_2INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_SERIES_HEADER_NAMELESS_INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_SERIES_HEADER_NOINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_SERIES_NOHEADER_2INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_SERIES_NOHEADER_INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_SERIES_NOHEADER_NOINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_STRING</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_TIMESERIES</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_TRANSPOSE</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_TRANSPOSE_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_VERTICAL_LIST</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_VERTICAL_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_READ_WORKBOOK_CALLER</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_RETURN_PD_NAT</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_VARIABLE_ARGS</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_2DLIST</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DATE</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DATETIME</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_0HEADER_0INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_0HEADER_1INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_0HEADER_2INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_1HEADER_0INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_1HEADER_1NAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_1HEADER_1UNNAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_1HEADER_2NAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_2HEADER_0INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_2HEADER_1NAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_2HEADER_1UNNAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_2HEADER_2NAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_2HEADER_2UNNAMEDINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DF_DATE_INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_DICT</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_FLOAT</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_HORIZONTAL_LIST</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_NONE</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_NP_SCALAR</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMED_2INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMED_INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMELESS_2INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMELESS_INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_SERIES_HEADER_NOINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_SERIES_NAN</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_SERIES_NOHEADER_2INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_SERIES_NOHEADER_INDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_SERIES_NOHEADER_NOINDEX</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_STRING</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_TIMESERIES</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_TRANSPOSE</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_TRANSPOSE_NPARRAY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGS_WRITE_VERTICAL_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_DEFAULT_ARGS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_EXPLICIT_DATE_FORMAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_METHOD_SIGNATURE_WITH_LESS_THAN_1024_CHARACTERS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_METHOD_SIGNATURE_WITH_MORE_THAN_1024_CHARACTERS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_NAMESPACE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_OPTIONAL_ARGS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_PARSE_DATES_INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_PARSE_DATES_NAMES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_PARSE_DATES_TRUE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_2DLIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DATE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DATE_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DATES_AS1</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DATES_AS2</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DATES_AS3</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DATES_AS_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DATETIME</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_0HEADER_0INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_0HEADER_1INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_0HEADER_2INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_1HEADER_0INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_1HEADER_1NAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_1HEADER_1UNNAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_1HEADER_2NAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_2HEADER_0INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_2HEADER_1NAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_2HEADER_1UNNAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_2HEADER_2NAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_2HEADER_2UNNAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DF_DATE_INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DICT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_DICT_TRANSPOSE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_EMPTY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_EMPTY_AS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_EMPTY_AS_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_EMPTY_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_ERROR_CELLS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_ERROR_CELLS_STR</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_FLOAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_HORIZONTAL_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_HORIZONTAL_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_NDIM1</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_NDIM1_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_NDIM2</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_NDIM2_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_SCALAR_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_SERIES_HEADER_NAMED_2INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_SERIES_HEADER_NAMED_INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_SERIES_HEADER_NAMELESS_2INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_SERIES_HEADER_NAMELESS_INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_SERIES_HEADER_NOINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_SERIES_NOHEADER_2INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_SERIES_NOHEADER_INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_SERIES_NOHEADER_NOINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_STRING</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_TIMESERIES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_TRANSPOSE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_TRANSPOSE_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_VERTICAL_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_VERTICAL_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_READ_WORKBOOK_CALLER</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_RETURN_PD_NAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_VARIABLE_ARGS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_VOLATILE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_2DLIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DATE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DATETIME</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_0HEADER_0INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_0HEADER_1INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_0HEADER_2INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_1HEADER_0INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_1HEADER_1NAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_1HEADER_1UNNAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_1HEADER_2NAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_2HEADER_0INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_2HEADER_1NAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_2HEADER_1UNNAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_2HEADER_2NAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_2HEADER_2UNNAMEDINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DF_DATE_INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_DICT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_ERROR_CELLS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_FLOAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_HORIZONTAL_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_NONE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_NP_SCALAR</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NAMED_2INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NAMED_INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NAMELESS_2INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NAMELESS_INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NOINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_SERIES_NAN</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_SERIES_NOHEADER_2INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_SERIES_NOHEADER_INDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_SERIES_NOHEADER_NOINDEX</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_STRING</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_TIMESERIES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_TRANSPOSE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_TRANSPOSE_NPARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_VERTICAL_LIST</we:customFunctionIds>
       </we:customFunctionIdList>
     </a:ext>
   </we:extLst>
@@ -1364,10 +1272,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P353"/>
+  <dimension ref="A1:P358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G355" sqref="G355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1380,8 +1288,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>110</v>
+      <c r="A1" s="25" t="s">
+        <v>123</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>0</v>
@@ -1415,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="b" cm="1">
-        <f t="array" ref="G6">_xldudf_XLWINGS_READ_FLOAT(2)</f>
+        <f t="array" ref="G6">_xldudf_XLWINGSJS_READ_FLOAT(2)</f>
         <v>1</v>
       </c>
       <c r="H6" t="b">
@@ -1431,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="b" cm="1">
-        <f t="array" ref="G7">[1]!_xldudf_XLWINGS_READ_FLOAT(D7)</f>
+        <f t="array" ref="G7">_xldudf_XLWINGSJS_READ_FLOAT(D7)</f>
         <v>1</v>
       </c>
       <c r="H7" t="b">
@@ -1452,7 +1360,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="2" cm="1">
-        <f t="array" ref="G9">[1]!_xldudf_XLWINGS_WRITE_FLOAT()</f>
+        <f t="array" ref="G9">_xldudf_XLWINGSJS_WRITE_FLOAT()</f>
         <v>2</v>
       </c>
       <c r="H9" t="b">
@@ -1473,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="2" t="b" cm="1">
-        <f t="array" ref="G11">[1]!_xldudf_XLWINGS_READ_STRING("xlwings")</f>
+        <f t="array" ref="G11">_xldudf_XLWINGSJS_READ_STRING("xlwings")</f>
         <v>1</v>
       </c>
       <c r="H11" t="b">
@@ -1489,7 +1397,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="b" cm="1">
-        <f t="array" ref="G12">[1]!_xldudf_XLWINGS_READ_STRING(D12)</f>
+        <f t="array" ref="G12">_xldudf_XLWINGSJS_READ_STRING(D12)</f>
         <v>1</v>
       </c>
       <c r="H12" t="b">
@@ -1510,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="2" t="str" cm="1">
-        <f t="array" ref="G14">[1]!_xldudf_XLWINGS_WRITE_STRING()</f>
+        <f t="array" ref="G14">_xldudf_XLWINGSJS_WRITE_STRING()</f>
         <v>xlwings</v>
       </c>
       <c r="H14" t="b">
@@ -1535,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="2" t="b" cm="1">
-        <f t="array" ref="G16">[1]!_xldudf_XLWINGS_READ_EMPTY(D16)</f>
+        <f t="array" ref="G16">_xldudf_XLWINGSJS_READ_EMPTY(D16)</f>
         <v>1</v>
       </c>
       <c r="H16" t="b">
@@ -1562,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="b" cm="1">
-        <f t="array" ref="G18">[1]!_xldudf_XLWINGS_READ_DATE(D18)</f>
+        <f t="array" ref="G18">_xldudf_XLWINGSJS_READ_DATE(D18)</f>
         <v>1</v>
       </c>
       <c r="H18" t="b">
@@ -1584,7 +1492,7 @@
         <v>25568</v>
       </c>
       <c r="G20" s="6" cm="1" vm="1">
-        <f t="array" ref="G20">[1]!_xldudf_XLWINGS_WRITE_DATE()</f>
+        <f t="array" ref="G20">_xldudf_XLWINGSJS_WRITE_DATE()</f>
         <v>25568</v>
       </c>
       <c r="H20" t="b">
@@ -1611,7 +1519,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="2" t="b" cm="1">
-        <f t="array" ref="G22">[1]!_xldudf_XLWINGS_READ_DATETIME(D22)</f>
+        <f t="array" ref="G22">_xldudf_XLWINGSJS_READ_DATETIME(D22)</f>
         <v>1</v>
       </c>
       <c r="H22" t="b">
@@ -1638,7 +1546,7 @@
         <v>27805.546099537038</v>
       </c>
       <c r="G24" s="16" cm="1" vm="2">
-        <f t="array" ref="G24">[1]!_xldudf_XLWINGS_WRITE_DATETIME()</f>
+        <f t="array" ref="G24">_xldudf_XLWINGSJS_WRITE_DATETIME()</f>
         <v>27805.546099537041</v>
       </c>
       <c r="H24" t="b">
@@ -1670,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="2" t="b" cm="1">
-        <f t="array" ref="G26">[1]!_xldudf_XLWINGS_READ_HORIZONTAL_LIST(D26:E26)</f>
+        <f t="array" ref="G26">_xldudf_XLWINGSJS_READ_HORIZONTAL_LIST(D26:E26)</f>
         <v>1</v>
       </c>
       <c r="H26" t="b">
@@ -1694,7 +1602,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="2" cm="1">
-        <f t="array" ref="G28:H28">[1]!_xldudf_XLWINGS_WRITE_HORIZONTAL_LIST()</f>
+        <f t="array" ref="G28:H28">_xldudf_XLWINGSJS_WRITE_HORIZONTAL_LIST()</f>
         <v>1</v>
       </c>
       <c r="H28" s="2">
@@ -1725,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="2" t="b" cm="1">
-        <f t="array" ref="G30">[1]!_xldudf_XLWINGS_READ_VERTICAL_LIST(D30:D31)</f>
+        <f t="array" ref="G30">_xldudf_XLWINGSJS_READ_VERTICAL_LIST(D30:D31)</f>
         <v>1</v>
       </c>
       <c r="H30" t="b">
@@ -1751,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="2" cm="1">
-        <f t="array" ref="G33:G34">[1]!_xldudf_XLWINGS_WRITE_VERTICAL_LIST()</f>
+        <f t="array" ref="G33:G34">_xldudf_XLWINGSJS_WRITE_VERTICAL_LIST()</f>
         <v>1</v>
       </c>
       <c r="H33" t="b">
@@ -1790,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="2" t="b" cm="1">
-        <f t="array" ref="G36">[1]!_xldudf_XLWINGS_READ_2DLIST(D36:E37)</f>
+        <f t="array" ref="G36">_xldudf_XLWINGSJS_READ_2DLIST(D36:E37)</f>
         <v>1</v>
       </c>
       <c r="H36" t="b">
@@ -1822,7 +1730,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="2" cm="1">
-        <f t="array" ref="G39:H40">[1]!_xldudf_XLWINGS_WRITE_2DLIST()</f>
+        <f t="array" ref="G39:H40">_xldudf_XLWINGSJS_WRITE_2DLIST()</f>
         <v>1</v>
       </c>
       <c r="H39" s="2">
@@ -1875,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="2" t="b" cm="1">
-        <f t="array" ref="G42">[1]!_xldudf_XLWINGS_READ_NDIM1(D42)</f>
+        <f t="array" ref="G42">_xldudf_XLWINGSJS_READ_NDIM1(D42)</f>
         <v>1</v>
       </c>
       <c r="H42" t="b">
@@ -1899,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="2" t="b" cm="1">
-        <f t="array" ref="G44">[1]!_xldudf_XLWINGS_READ_NDIM2(D44)</f>
+        <f t="array" ref="G44">_xldudf_XLWINGSJS_READ_NDIM2(D44)</f>
         <v>1</v>
       </c>
       <c r="H44" t="b">
@@ -1926,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="2" t="b" cm="1">
-        <f t="array" ref="G46">[1]!_xldudf_XLWINGS_READ_TRANSPOSE(D46:E47)</f>
+        <f t="array" ref="G46">_xldudf_XLWINGSJS_READ_TRANSPOSE(D46:E47)</f>
         <v>1</v>
       </c>
       <c r="H46" t="b">
@@ -1958,7 +1866,7 @@
         <v>3</v>
       </c>
       <c r="G49" s="2" cm="1">
-        <f t="array" ref="G49:H50">[1]!_xldudf_XLWINGS_WRITE_TRANSPOSE()</f>
+        <f t="array" ref="G49:H50">_xldudf_XLWINGSJS_WRITE_TRANSPOSE()</f>
         <v>1</v>
       </c>
       <c r="H49" s="2">
@@ -2014,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="2" t="b" cm="1">
-        <f t="array" ref="G52">[1]!_xldudf_XLWINGS_READ_DATES_AS1(D52:E53)</f>
+        <f t="array" ref="G52">_xldudf_XLWINGSJS_READ_DATES_AS1(D52:E53)</f>
         <v>1</v>
       </c>
       <c r="H52" t="b">
@@ -2050,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="2" t="b" cm="1">
-        <f t="array" ref="G55">[1]!_xldudf_XLWINGS_READ_DATES_AS2(E55)</f>
+        <f t="array" ref="G55">_xldudf_XLWINGSJS_READ_DATES_AS2(E55)</f>
         <v>1</v>
       </c>
       <c r="H55" t="b">
@@ -2080,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="2" t="b" cm="1">
-        <f t="array" ref="G58">[1]!_xldudf_XLWINGS_READ_DATES_AS3(D58:E59)</f>
+        <f t="array" ref="G58">_xldudf_XLWINGSJS_READ_DATES_AS3(D58:E59)</f>
         <v>1</v>
       </c>
       <c r="H58" t="b">
@@ -2116,7 +2024,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="2" t="b" cm="1">
-        <f t="array" ref="G61">[1]!_xldudf_XLWINGS_READ_EMPTY_AS(D61:E62)</f>
+        <f t="array" ref="G61">_xldudf_XLWINGSJS_READ_EMPTY_AS(D61:E62)</f>
         <v>1</v>
       </c>
       <c r="H61" t="b">
@@ -2155,7 +2063,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="2" t="b" cm="1">
-        <f t="array" ref="G64">[1]!_xldudf_XLWINGS_READ_DICT(D64:E65)</f>
+        <f t="array" ref="G64">_xldudf_XLWINGSJS_READ_DICT(D64:E65)</f>
         <v>1</v>
       </c>
       <c r="H64" t="b">
@@ -2190,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="2" t="b" cm="1">
-        <f t="array" ref="G67">[1]!_xldudf_XLWINGS_READ_DICT_TRANSPOSE(D67:E68)</f>
+        <f t="array" ref="G67">_xldudf_XLWINGSJS_READ_DICT_TRANSPOSE(D67:E68)</f>
         <v>1</v>
       </c>
       <c r="H67" t="b">
@@ -2222,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="11" t="str" cm="1">
-        <f t="array" ref="G70:H71">[1]!_xldudf_XLWINGS_WRITE_DICT()</f>
+        <f t="array" ref="G70:H71">_xldudf_XLWINGSJS_WRITE_DICT()</f>
         <v>a</v>
       </c>
       <c r="H70" s="11">
@@ -2275,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="2" t="b">
-        <f>[1]!_xldudf_XLWINGS_READ_SCALAR_NPARRAY(D73)</f>
+        <f>_xldudf_XLWINGSJS_READ_SCALAR_NPARRAY(D73)</f>
         <v>1</v>
       </c>
       <c r="H73" t="b">
@@ -2300,7 +2208,7 @@
         <v>1</v>
       </c>
       <c r="G75" s="2" t="b" cm="1">
-        <f t="array" ref="G75">[1]!_xldudf_XLWINGS_READ_EMPTY_NPARRAY(D76)</f>
+        <f t="array" ref="G75">_xldudf_XLWINGSJS_READ_EMPTY_NPARRAY(D76)</f>
         <v>1</v>
       </c>
       <c r="H75" t="b">
@@ -2335,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="2" t="b" cm="1">
-        <f t="array" ref="G77">[1]!_xldudf_XLWINGS_READ_HORIZONTAL_NPARRAY(D77:E77)</f>
+        <f t="array" ref="G77">_xldudf_XLWINGSJS_READ_HORIZONTAL_NPARRAY(D77:E77)</f>
         <v>1</v>
       </c>
       <c r="H77" t="b">
@@ -2359,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="G79" s="2" t="b" cm="1">
-        <f t="array" ref="G79">[1]!_xldudf_XLWINGS_READ_VERTICAL_NPARRAY(D79:D80)</f>
+        <f t="array" ref="G79">_xldudf_XLWINGSJS_READ_VERTICAL_NPARRAY(D79:D80)</f>
         <v>1</v>
       </c>
       <c r="H79" t="b">
@@ -2388,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="G82" s="2" t="b" cm="1">
-        <f t="array" ref="G82">[1]!_xldudf_XLWINGS_READ_NDIM1_NPARRAY(D82)</f>
+        <f t="array" ref="G82">_xldudf_XLWINGSJS_READ_NDIM1_NPARRAY(D82)</f>
         <v>1</v>
       </c>
       <c r="H82" t="b">
@@ -2412,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="2" t="b" cm="1">
-        <f t="array" ref="G84">[1]!_xldudf_XLWINGS_READ_NDIM2_NPARRAY(D84)</f>
+        <f t="array" ref="G84">_xldudf_XLWINGSJS_READ_NDIM2_NPARRAY(D84)</f>
         <v>1</v>
       </c>
       <c r="H84" t="b">
@@ -2439,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="2" t="b" cm="1">
-        <f t="array" ref="G86">[1]!_xldudf_XLWINGS_READ_TRANSPOSE_NPARRAY(D86:E87)</f>
+        <f t="array" ref="G86">_xldudf_XLWINGSJS_READ_TRANSPOSE_NPARRAY(D86:E87)</f>
         <v>1</v>
       </c>
       <c r="H86" t="b">
@@ -2471,7 +2379,7 @@
         <v>3</v>
       </c>
       <c r="G89" s="2" cm="1">
-        <f t="array" ref="G89:H90">[1]!_xldudf_XLWINGS_WRITE_TRANSPOSE_NPARRAY()</f>
+        <f t="array" ref="G89:H90">_xldudf_XLWINGSJS_WRITE_TRANSPOSE_NPARRAY()</f>
         <v>1</v>
       </c>
       <c r="H89" s="2">
@@ -2524,7 +2432,7 @@
         <v>1</v>
       </c>
       <c r="G92" s="2" t="b" cm="1">
-        <f t="array" ref="G92">[1]!_xldudf_XLWINGS_READ_DATE_NPARRAY(D92)</f>
+        <f t="array" ref="G92">_xldudf_XLWINGSJS_READ_DATE_NPARRAY(D92)</f>
         <v>1</v>
       </c>
       <c r="H92" t="b">
@@ -2548,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="G94" s="2" t="b" cm="1">
-        <f t="array" ref="G94">[1]!_xldudf_XLWINGS_READ_DATES_AS_NPARRAY(D94)</f>
+        <f t="array" ref="G94">_xldudf_XLWINGSJS_READ_DATES_AS_NPARRAY(D94)</f>
         <v>1</v>
       </c>
       <c r="H94" t="b">
@@ -2573,7 +2481,7 @@
         <v>1</v>
       </c>
       <c r="G96" s="2" t="b" cm="1">
-        <f t="array" ref="G96">[1]!_xldudf_XLWINGS_READ_EMPTY_AS_NPARRAY(D96)</f>
+        <f t="array" ref="G96">_xldudf_XLWINGSJS_READ_EMPTY_AS_NPARRAY(D96)</f>
         <v>1</v>
       </c>
       <c r="H96" t="b">
@@ -2598,7 +2506,7 @@
         <v>2</v>
       </c>
       <c r="G98" s="2" cm="1">
-        <f t="array" ref="G98">[1]!_xldudf_XLWINGS_WRITE_NP_SCALAR()</f>
+        <f t="array" ref="G98">_xldudf_XLWINGSJS_WRITE_NP_SCALAR()</f>
         <v>2</v>
       </c>
       <c r="H98" t="b">
@@ -2626,7 +2534,7 @@
         <v>1</v>
       </c>
       <c r="G100" s="2" t="b" cm="1">
-        <f t="array" ref="G100">[1]!_xldudf_XLWINGS_READ_SERIES_NOHEADER_NOINDEX(D100:D101)</f>
+        <f t="array" ref="G100">_xldudf_XLWINGSJS_READ_SERIES_NOHEADER_NOINDEX(D100:D101)</f>
         <v>1</v>
       </c>
       <c r="H100" t="b">
@@ -2661,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="G103" s="2" t="b" cm="1">
-        <f t="array" ref="G103">[1]!_xldudf_XLWINGS_READ_SERIES_NOHEADER_INDEX(D103:E104)</f>
+        <f t="array" ref="G103">_xldudf_XLWINGSJS_READ_SERIES_NOHEADER_INDEX(D103:E104)</f>
         <v>1</v>
       </c>
       <c r="H103" t="b">
@@ -2693,7 +2601,7 @@
         <v>1</v>
       </c>
       <c r="G106" s="2" t="b" cm="1">
-        <f t="array" ref="G106">[1]!_xldudf_XLWINGS_READ_SERIES_HEADER_NOINDEX(E106:E108)</f>
+        <f t="array" ref="G106">_xldudf_XLWINGSJS_READ_SERIES_HEADER_NOINDEX(E106:E108)</f>
         <v>1</v>
       </c>
       <c r="H106" t="b">
@@ -2730,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="G110" s="2" t="b" cm="1">
-        <f t="array" ref="G110">[1]!_xldudf_XLWINGS_READ_SERIES_HEADER_NAMED_INDEX(D110:E112)</f>
+        <f t="array" ref="G110">_xldudf_XLWINGSJS_READ_SERIES_HEADER_NAMED_INDEX(D110:E112)</f>
         <v>1</v>
       </c>
       <c r="H110" t="b">
@@ -2774,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="G114" s="2" t="b" cm="1">
-        <f t="array" ref="G114">[1]!_xldudf_XLWINGS_READ_SERIES_HEADER_NAMELESS_INDEX(D114:E116)</f>
+        <f t="array" ref="G114">_xldudf_XLWINGSJS_READ_SERIES_HEADER_NAMELESS_INDEX(D114:E116)</f>
         <v>1</v>
       </c>
       <c r="H114" t="b">
@@ -2811,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="G118" s="2" cm="1">
-        <f t="array" ref="G118:G119">[1]!_xldudf_XLWINGS_WRITE_SERIES_NOHEADER_NOINDEX()</f>
+        <f t="array" ref="G118:G119">_xldudf_XLWINGSJS_WRITE_SERIES_NOHEADER_NOINDEX()</f>
         <v>1</v>
       </c>
       <c r="H118" t="b">
@@ -2847,7 +2755,7 @@
         <v>1</v>
       </c>
       <c r="G121" s="2" cm="1">
-        <f t="array" ref="G121:H122">[1]!_xldudf_XLWINGS_WRITE_SERIES_NOHEADER_INDEX()</f>
+        <f t="array" ref="G121:H122">_xldudf_XLWINGSJS_WRITE_SERIES_NOHEADER_INDEX()</f>
         <v>10</v>
       </c>
       <c r="H121" s="2">
@@ -2897,7 +2805,7 @@
         <v>3</v>
       </c>
       <c r="G124" s="11" t="str" cm="1">
-        <f t="array" ref="G124:G126">[1]!_xldudf_XLWINGS_WRITE_SERIES_HEADER_NOINDEX()</f>
+        <f t="array" ref="G124:G126">_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NOINDEX()</f>
         <v>name</v>
       </c>
       <c r="H124" t="b">
@@ -2945,7 +2853,7 @@
         <v>3</v>
       </c>
       <c r="G128" s="11" t="str" cm="1">
-        <f t="array" ref="G128:H130">[1]!_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMED_INDEX()</f>
+        <f t="array" ref="G128:H130">_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NAMED_INDEX()</f>
         <v>ix</v>
       </c>
       <c r="H128" s="11" t="str">
@@ -3018,7 +2926,7 @@
         <v>3</v>
       </c>
       <c r="G132" s="2" t="str" cm="1">
-        <f t="array" ref="G132:H134">[1]!_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMELESS_INDEX()</f>
+        <f t="array" ref="G132:H134">_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NAMELESS_INDEX()</f>
         <v/>
       </c>
       <c r="H132" s="2" t="str">
@@ -3097,7 +3005,7 @@
         <v>1</v>
       </c>
       <c r="G136" s="2" t="b" cm="1">
-        <f t="array" ref="G136">[1]!_xldudf_XLWINGS_READ_TIMESERIES(D136:E138)</f>
+        <f t="array" ref="G136">_xldudf_XLWINGSJS_READ_TIMESERIES(D136:E138)</f>
         <v>1</v>
       </c>
       <c r="H136" t="b">
@@ -3141,7 +3049,7 @@
         <v>48</v>
       </c>
       <c r="G140" s="11" t="str" cm="1">
-        <f t="array" ref="G140:H142">[1]!_xldudf_XLWINGS_WRITE_TIMESERIES()</f>
+        <f t="array" ref="G140:H142">_xldudf_XLWINGSJS_WRITE_TIMESERIES()</f>
         <v/>
       </c>
       <c r="H140" s="11" t="str">
@@ -3219,7 +3127,7 @@
         <v>1</v>
       </c>
       <c r="G144" s="2" t="b" cm="1">
-        <f t="array" ref="G144">[1]!_xldudf_XLWINGS_READ_DF_0HEADER_0INDEX(D144:E145)</f>
+        <f t="array" ref="G144">_xldudf_XLWINGSJS_READ_DF_0HEADER_0INDEX(D144:E145)</f>
         <v>1</v>
       </c>
       <c r="H144" t="b">
@@ -3251,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="G147" s="2" cm="1">
-        <f t="array" ref="G147:H148">[1]!_xldudf_XLWINGS_WRITE_DF_0HEADER_0INDEX()</f>
+        <f t="array" ref="G147:H148">_xldudf_XLWINGSJS_WRITE_DF_0HEADER_0INDEX()</f>
         <v>1</v>
       </c>
       <c r="H147" s="2">
@@ -3306,7 +3214,7 @@
         <v>1</v>
       </c>
       <c r="G150" s="2" t="b" cm="1">
-        <f t="array" ref="G150">[1]!_xldudf_XLWINGS_READ_DF_1HEADER_0INDEX(D150:E152)</f>
+        <f t="array" ref="G150">_xldudf_XLWINGSJS_READ_DF_1HEADER_0INDEX(D150:E152)</f>
         <v>1</v>
       </c>
       <c r="H150" t="b">
@@ -3345,7 +3253,7 @@
         <v>51</v>
       </c>
       <c r="G154" s="11" t="str" cm="1">
-        <f t="array" ref="G154:H156">[1]!_xldudf_XLWINGS_WRITE_DF_1HEADER_0INDEX()</f>
+        <f t="array" ref="G154:H156">_xldudf_XLWINGSJS_WRITE_DF_1HEADER_0INDEX()</f>
         <v>a</v>
       </c>
       <c r="H154" s="11" t="str">
@@ -3425,7 +3333,7 @@
         <v>1</v>
       </c>
       <c r="G158" s="2" t="b" cm="1">
-        <f t="array" ref="G158">[1]!_xldudf_XLWINGS_READ_DF_0HEADER_1INDEX(C158:E159)</f>
+        <f t="array" ref="G158">_xldudf_XLWINGSJS_READ_DF_0HEADER_1INDEX(C158:E159)</f>
         <v>1</v>
       </c>
       <c r="H158" t="b">
@@ -3462,7 +3370,7 @@
         <v>2</v>
       </c>
       <c r="G161" s="2" cm="1">
-        <f t="array" ref="G161:I162">[1]!_xldudf_XLWINGS_WRITE_DF_0HEADER_1INDEX()</f>
+        <f t="array" ref="G161:I162">_xldudf_XLWINGSJS_WRITE_DF_0HEADER_1INDEX()</f>
         <v>10</v>
       </c>
       <c r="H161" s="11">
@@ -3535,7 +3443,7 @@
         <v>1</v>
       </c>
       <c r="G164" s="2" t="b" cm="1">
-        <f t="array" ref="G164">[1]!_xldudf_XLWINGS_READ_DF_0HEADER_2INDEX(B166:F168)</f>
+        <f t="array" ref="G164">_xldudf_XLWINGSJS_READ_DF_0HEADER_2INDEX(B166:F168)</f>
         <v>1</v>
       </c>
       <c r="H164" t="b">
@@ -3648,7 +3556,7 @@
         <v>3</v>
       </c>
       <c r="G171" s="2" t="str" cm="1">
-        <f t="array" ref="G171:K173">[1]!_xldudf_XLWINGS_WRITE_DF_0HEADER_2INDEX()</f>
+        <f t="array" ref="G171:K173">_xldudf_XLWINGSJS_WRITE_DF_0HEADER_2INDEX()</f>
         <v>a</v>
       </c>
       <c r="H171" s="11">
@@ -3809,7 +3717,7 @@
         <v>1</v>
       </c>
       <c r="G175" s="2" t="b" cm="1">
-        <f t="array" ref="G175">[1]!_xldudf_XLWINGS_READ_DF_1HEADER_1NAMEDINDEX(B176:E178)</f>
+        <f t="array" ref="G175">_xldudf_XLWINGSJS_READ_DF_1HEADER_1NAMEDINDEX(B176:E178)</f>
         <v>1</v>
       </c>
       <c r="H175" t="b">
@@ -3886,7 +3794,7 @@
         <v>52</v>
       </c>
       <c r="G180" s="11" t="str" cm="1">
-        <f t="array" ref="G180:J182">[1]!_xldudf_XLWINGS_WRITE_DF_1HEADER_1NAMEDINDEX()</f>
+        <f t="array" ref="G180:J182">_xldudf_XLWINGSJS_WRITE_DF_1HEADER_1NAMEDINDEX()</f>
         <v>ix1</v>
       </c>
       <c r="H180" s="11" t="str">
@@ -4016,7 +3924,7 @@
         <v>1</v>
       </c>
       <c r="G184" s="2" t="b" cm="1">
-        <f t="array" ref="G184">[1]!_xldudf_XLWINGS_READ_DF_1HEADER_1UNNAMEDINDEX(B185:E187)</f>
+        <f t="array" ref="G184">_xldudf_XLWINGSJS_READ_DF_1HEADER_1UNNAMEDINDEX(B185:E187)</f>
         <v>1</v>
       </c>
       <c r="H184" t="b">
@@ -4095,7 +4003,7 @@
         <v>52</v>
       </c>
       <c r="G189" s="11" t="str" cm="1">
-        <f t="array" ref="G189:J191">[1]!_xldudf_XLWINGS_WRITE_DF_1HEADER_1UNNAMEDINDEX()</f>
+        <f t="array" ref="G189:J191">_xldudf_XLWINGSJS_WRITE_DF_1HEADER_1UNNAMEDINDEX()</f>
         <v/>
       </c>
       <c r="H189" s="11" t="str">
@@ -4236,7 +4144,7 @@
         <v>1</v>
       </c>
       <c r="G193" s="2" t="b" cm="1">
-        <f t="array" ref="G193">[1]!_xldudf_XLWINGS_READ_DF_2HEADER_0INDEX(C194:E197)</f>
+        <f t="array" ref="G193">_xldudf_XLWINGSJS_READ_DF_2HEADER_0INDEX(C194:E197)</f>
         <v>1</v>
       </c>
       <c r="H193" s="8" t="b">
@@ -4336,7 +4244,7 @@
         <v>51</v>
       </c>
       <c r="G199" s="11" t="str" cm="1">
-        <f t="array" ref="G199:I202">[1]!_xldudf_XLWINGS_WRITE_DF_2HEADER_0INDEX()</f>
+        <f t="array" ref="G199:I202">_xldudf_XLWINGSJS_WRITE_DF_2HEADER_0INDEX()</f>
         <v>a</v>
       </c>
       <c r="H199" s="11" t="str">
@@ -4472,7 +4380,7 @@
         <v>1</v>
       </c>
       <c r="G204" s="2" t="b" cm="1">
-        <f t="array" ref="G204">[1]!_xldudf_XLWINGS_READ_DF_2HEADER_1NAMEDINDEX(B205:E208)</f>
+        <f t="array" ref="G204">_xldudf_XLWINGSJS_READ_DF_2HEADER_1NAMEDINDEX(B205:E208)</f>
         <v>1</v>
       </c>
       <c r="H204" t="b">
@@ -4565,7 +4473,7 @@
         <v>51</v>
       </c>
       <c r="G210" s="11" t="str" cm="1">
-        <f t="array" ref="G210:J213">[1]!_xldudf_XLWINGS_WRITE_DF_2HEADER_1NAMEDINDEX()</f>
+        <f t="array" ref="G210:J213">_xldudf_XLWINGSJS_WRITE_DF_2HEADER_1NAMEDINDEX()</f>
         <v/>
       </c>
       <c r="H210" s="11" t="str">
@@ -4732,7 +4640,7 @@
         <v>1</v>
       </c>
       <c r="G215" s="2" t="b" cm="1">
-        <f t="array" ref="G215">[1]!_xldudf_XLWINGS_READ_DF_2HEADER_1UNNAMEDINDEX(B216:E219)</f>
+        <f t="array" ref="G215">_xldudf_XLWINGSJS_READ_DF_2HEADER_1UNNAMEDINDEX(B216:E219)</f>
         <v>1</v>
       </c>
       <c r="H215" t="b">
@@ -4826,7 +4734,7 @@
         <v>51</v>
       </c>
       <c r="G221" s="11" t="str" cm="1">
-        <f t="array" ref="G221:J224">[1]!_xldudf_XLWINGS_WRITE_DF_2HEADER_1UNNAMEDINDEX()</f>
+        <f t="array" ref="G221:J224">_xldudf_XLWINGSJS_WRITE_DF_2HEADER_1UNNAMEDINDEX()</f>
         <v/>
       </c>
       <c r="H221" s="11" t="str">
@@ -4997,7 +4905,7 @@
         <v>1</v>
       </c>
       <c r="G226" s="2" t="b" cm="1">
-        <f t="array" ref="G226">[1]!_xldudf_XLWINGS_READ_DF_2HEADER_2NAMEDINDEX(B227:F231)</f>
+        <f t="array" ref="G226">_xldudf_XLWINGSJS_READ_DF_2HEADER_2NAMEDINDEX(B227:F231)</f>
         <v>1</v>
       </c>
       <c r="H226" t="b">
@@ -5131,7 +5039,7 @@
         <v>51</v>
       </c>
       <c r="G234" s="11" t="str" cm="1">
-        <f t="array" ref="G234:K238">[1]!_xldudf_XLWINGS_WRITE_DF_2HEADER_2NAMEDINDEX()</f>
+        <f t="array" ref="G234:K238">_xldudf_XLWINGSJS_WRITE_DF_2HEADER_2NAMEDINDEX()</f>
         <v/>
       </c>
       <c r="H234" s="11" t="str">
@@ -5394,7 +5302,7 @@
         <v>1</v>
       </c>
       <c r="G242" s="2" t="b" cm="1">
-        <f t="array" ref="G242">[1]!_xldudf_XLWINGS_READ_DF_2HEADER_2UNNAMEDINDEX(B243:F247)</f>
+        <f t="array" ref="G242">_xldudf_XLWINGSJS_READ_DF_2HEADER_2UNNAMEDINDEX(B243:F247)</f>
         <v>1</v>
       </c>
       <c r="H242" t="b">
@@ -5530,7 +5438,7 @@
         <v>51</v>
       </c>
       <c r="G250" s="11" t="str" cm="1">
-        <f t="array" ref="G250:K254">[1]!_xldudf_XLWINGS_WRITE_DF_2HEADER_2UNNAMEDINDEX()</f>
+        <f t="array" ref="G250:K254">_xldudf_XLWINGSJS_WRITE_DF_2HEADER_2UNNAMEDINDEX()</f>
         <v/>
       </c>
       <c r="H250" s="11" t="str">
@@ -5788,7 +5696,7 @@
         <v>1</v>
       </c>
       <c r="G256" s="2" t="b" cm="1">
-        <f t="array" ref="G256">[1]!_xldudf_XLWINGS_READ_DF_1HEADER_2NAMEDINDEX(B257:F260)</f>
+        <f t="array" ref="G256">_xldudf_XLWINGSJS_READ_DF_1HEADER_2NAMEDINDEX(B257:F260)</f>
         <v>1</v>
       </c>
       <c r="H256" t="b">
@@ -5897,7 +5805,7 @@
         <v>52</v>
       </c>
       <c r="G263" s="11" t="str" cm="1">
-        <f t="array" ref="G263:K266">[1]!_xldudf_XLWINGS_WRITE_DF_1HEADER_2NAMEDINDEX()</f>
+        <f t="array" ref="G263:K266">_xldudf_XLWINGSJS_WRITE_DF_1HEADER_2NAMEDINDEX()</f>
         <v>x1</v>
       </c>
       <c r="H263" s="11" t="str">
@@ -6113,7 +6021,7 @@
         <v>1</v>
       </c>
       <c r="G268" s="2" t="b" cm="1">
-        <f t="array" ref="G268">[1]!_xldudf_XLWINGS_READ_DF_DATE_INDEX(B269:E271)</f>
+        <f t="array" ref="G268">_xldudf_XLWINGSJS_READ_DF_DATE_INDEX(B269:E271)</f>
         <v>1</v>
       </c>
       <c r="H268" t="b">
@@ -6186,7 +6094,7 @@
         <v>52</v>
       </c>
       <c r="G273" s="11" t="str" cm="1">
-        <f t="array" ref="G273:J275">[1]!_xldudf_XLWINGS_WRITE_DF_DATE_INDEX()</f>
+        <f t="array" ref="G273:J275">_xldudf_XLWINGSJS_WRITE_DF_DATE_INDEX()</f>
         <v/>
       </c>
       <c r="H273" s="11" t="str">
@@ -6311,7 +6219,7 @@
         <v>153</v>
       </c>
       <c r="G277" s="2" cm="1">
-        <f t="array" ref="G277">[1]!_xldudf_XLWINGS_DEFAULT_ARGS(2,"bye")</f>
+        <f t="array" ref="G277">_xldudf_XLWINGSJS_DEFAULT_ARGS(2,"bye")</f>
         <v>153</v>
       </c>
       <c r="H277" t="b">
@@ -6331,7 +6239,7 @@
         <v>153</v>
       </c>
       <c r="G279" s="2" cm="1">
-        <f t="array" ref="G279">[1]!_xldudf_XLWINGS_VARIABLE_ARGS(2, 20, 30, 40)</f>
+        <f t="array" ref="G279">_xldudf_XLWINGSJS_VARIABLE_ARGS(2, 20, 30, 40)</f>
         <v>153</v>
       </c>
       <c r="H279" t="b">
@@ -6351,7 +6259,7 @@
         <v>20</v>
       </c>
       <c r="G281" s="2" cm="1">
-        <f t="array" ref="G281">[1]!_xldudf_XLWINGS_OPTIONAL_ARGS(2)</f>
+        <f t="array" ref="G281">_xldudf_XLWINGSJS_OPTIONAL_ARGS(2)</f>
         <v>20</v>
       </c>
       <c r="H281" t="b">
@@ -6360,12 +6268,20 @@
       </c>
     </row>
     <row r="282" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A282" t="b">
+        <f>H282</f>
+        <v>1</v>
+      </c>
       <c r="F282" s="1">
         <v>30</v>
       </c>
       <c r="G282" s="2" cm="1">
-        <f t="array" ref="G282">[1]!_xldudf_XLWINGS_OPTIONAL_ARGS(1, 30)</f>
+        <f t="array" ref="G282">_xldudf_XLWINGSJS_OPTIONAL_ARGS(1, 30)</f>
         <v>30</v>
+      </c>
+      <c r="H282" t="b">
+        <f>G282=F282</f>
+        <v>1</v>
       </c>
     </row>
     <row r="284" spans="1:14" x14ac:dyDescent="0.2">
@@ -6378,7 +6294,7 @@
       </c>
       <c r="F284" s="1"/>
       <c r="G284" s="2" t="str" cm="1">
-        <f t="array" ref="G284">[1]!_xldudf_XLWINGS_WRITE_NONE()</f>
+        <f t="array" ref="G284">_xldudf_XLWINGSJS_WRITE_NONE()</f>
         <v/>
       </c>
       <c r="H284" t="b">
@@ -6399,7 +6315,7 @@
         <v>1</v>
       </c>
       <c r="G286" s="2" t="b" cm="1">
-        <f t="array" ref="G286">[1]!_xldudf_XLWINGS_READ_SERIES_HEADER_NAMELESS_2INDEX(C287:E289)</f>
+        <f t="array" ref="G286">_xldudf_XLWINGSJS_READ_SERIES_HEADER_NAMELESS_2INDEX(C287:E289)</f>
         <v>1</v>
       </c>
       <c r="H286" t="b">
@@ -6455,7 +6371,7 @@
         <v>1</v>
       </c>
       <c r="G291" s="2" t="b" cm="1">
-        <f t="array" ref="G291">[1]!_xldudf_XLWINGS_READ_SERIES_HEADER_NAMED_2INDEX(C292:E294)</f>
+        <f t="array" ref="G291">_xldudf_XLWINGSJS_READ_SERIES_HEADER_NAMED_2INDEX(C292:E294)</f>
         <v>1</v>
       </c>
       <c r="H291" t="b">
@@ -6509,7 +6425,7 @@
         <v>1</v>
       </c>
       <c r="G295" s="2" t="b" cm="1">
-        <f t="array" ref="G295">[1]!_xldudf_XLWINGS_READ_SERIES_NOHEADER_2INDEX(C296:E297)</f>
+        <f t="array" ref="G295">_xldudf_XLWINGSJS_READ_SERIES_NOHEADER_2INDEX(C296:E297)</f>
         <v>1</v>
       </c>
       <c r="H295" t="b">
@@ -6560,7 +6476,7 @@
         <v>3</v>
       </c>
       <c r="G299" s="11" t="str" cm="1">
-        <f t="array" ref="G299:I301">[1]!_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMELESS_2INDEX()</f>
+        <f t="array" ref="G299:I301">_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NAMELESS_2INDEX()</f>
         <v/>
       </c>
       <c r="H299" s="11" t="str">
@@ -6670,7 +6586,7 @@
         <v>3</v>
       </c>
       <c r="G303" s="11" t="str" cm="1">
-        <f t="array" ref="G303:I305">[1]!_xldudf_XLWINGS_WRITE_SERIES_HEADER_NAMED_2INDEX()</f>
+        <f t="array" ref="G303:I305">_xldudf_XLWINGSJS_WRITE_SERIES_HEADER_NAMED_2INDEX()</f>
         <v>ix1</v>
       </c>
       <c r="H303" s="11" t="str">
@@ -6780,7 +6696,7 @@
         <v>1</v>
       </c>
       <c r="G307" s="11" t="str" cm="1">
-        <f t="array" ref="G307:I308">[1]!_xldudf_XLWINGS_WRITE_SERIES_NOHEADER_2INDEX()</f>
+        <f t="array" ref="G307:I308">_xldudf_XLWINGSJS_WRITE_SERIES_NOHEADER_2INDEX()</f>
         <v>a</v>
       </c>
       <c r="H307" s="11">
@@ -6850,7 +6766,7 @@
         <v>1</v>
       </c>
       <c r="G310" s="22" cm="1">
-        <f t="array" ref="G310:G312">[1]!_xldudf_XLWINGS_WRITE_SERIES_NAN()</f>
+        <f t="array" ref="G310:G312">_xldudf_XLWINGSJS_WRITE_SERIES_NAN()</f>
         <v>1</v>
       </c>
       <c r="H310" s="8"/>
@@ -6885,7 +6801,7 @@
         <v>3</v>
       </c>
       <c r="K312" t="b">
-        <f t="shared" ref="K311:K312" si="59">G312=F312</f>
+        <f t="shared" ref="K312" si="59">G312=F312</f>
         <v>1</v>
       </c>
     </row>
@@ -6901,7 +6817,7 @@
         <v>102</v>
       </c>
       <c r="G314" s="2" t="str" cm="1">
-        <f t="array" ref="G314">[1]!_xldudf_XLWINGS_METHOD_SIGNATURE_WITH_MORE_THAN_1024_CHARACTERS()</f>
+        <f t="array" ref="G314">_xldudf_XLWINGSJS_METHOD_SIGNATURE_WITH_MORE_THAN_1024_CHARACTERS()</f>
         <v>splitted signature</v>
       </c>
       <c r="H314" t="b">
@@ -6921,7 +6837,7 @@
         <v>104</v>
       </c>
       <c r="G316" s="2" t="str" cm="1">
-        <f t="array" ref="G316">[1]!_xldudf_XLWINGS_METHOD_SIGNATURE_WITH_LESS_THAN_1024_CHARACTERS()</f>
+        <f t="array" ref="G316">_xldudf_XLWINGSJS_METHOD_SIGNATURE_WITH_LESS_THAN_1024_CHARACTERS()</f>
         <v>non splitted signature</v>
       </c>
       <c r="H316" t="b">
@@ -6942,7 +6858,7 @@
         <v>1</v>
       </c>
       <c r="G318" s="24" t="str" cm="1">
-        <f t="array" ref="G318:H319">[1]!_xldudf_XLWINGS_RETURN_PD_NAT()</f>
+        <f t="array" ref="G318:H319">_xldudf_XLWINGSJS_RETURN_PD_NAT()</f>
         <v/>
       </c>
       <c r="H318" s="24">
@@ -6983,23 +6899,23 @@
         <v>1</v>
       </c>
       <c r="B321" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C321" s="1" t="str">
         <f>""</f>
         <v/>
       </c>
       <c r="D321" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E321" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E321" s="1" t="s">
+      <c r="F321" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F321" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="G321" s="2" t="b" cm="1">
-        <f t="array" ref="G321">_xldudf_XLWINGS_PARSE_DATES_INDEX(C321:F324)</f>
+        <f t="array" ref="G321">_xldudf_XLWINGSJS_PARSE_DATES_INDEX(C321:F324)</f>
         <v>1</v>
       </c>
     </row>
@@ -7051,22 +6967,22 @@
         <v>1</v>
       </c>
       <c r="B326" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D326" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E326" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E326" s="1" t="s">
+      <c r="F326" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F326" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="G326" s="2" t="b" cm="1">
-        <f t="array" ref="G326">_xldudf_XLWINGS_PARSE_DATES_NAMES(C326:F329)</f>
+        <f t="array" ref="G326">_xldudf_XLWINGSJS_PARSE_DATES_NAMES(C326:F329)</f>
         <v>1</v>
       </c>
     </row>
@@ -7118,25 +7034,22 @@
         <v>1</v>
       </c>
       <c r="B332" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C332" s="25"/>
-      <c r="D332" s="25"/>
+        <v>114</v>
+      </c>
       <c r="E332" s="1" t="str">
         <f>""</f>
         <v/>
       </c>
       <c r="F332" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G332" s="2" t="b" cm="1">
-        <f t="array" ref="G332">_xldudf_XLWINGS_PARSE_DATES_TRUE(E332:F335)</f>
+        <f t="array" ref="G332">_xldudf_XLWINGSJS_PARSE_DATES_TRUE(E332:F335)</f>
         <v>1</v>
       </c>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C333" s="26"/>
-      <c r="D333" s="25"/>
+      <c r="C333" s="4"/>
       <c r="E333" s="5">
         <v>44197.466099537036</v>
       </c>
@@ -7145,8 +7058,7 @@
       </c>
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C334" s="26"/>
-      <c r="D334" s="25"/>
+      <c r="C334" s="4"/>
       <c r="E334" s="5">
         <v>44198.932199074072</v>
       </c>
@@ -7155,8 +7067,7 @@
       </c>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C335" s="26"/>
-      <c r="D335" s="25"/>
+      <c r="C335" s="4"/>
       <c r="E335" s="5">
         <v>44199</v>
       </c>
@@ -7170,10 +7081,10 @@
         <v>1</v>
       </c>
       <c r="B337" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G337" s="2" t="e" cm="1">
-        <f t="array" ref="G337:G343">_xldudf_XLWINGS_WRITE_ERROR_CELLS()</f>
+        <f t="array" ref="G337:G343">_xldudf_XLWINGSJS_WRITE_ERROR_CELLS()</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H337" t="b">
@@ -7241,10 +7152,10 @@
         <v>1</v>
       </c>
       <c r="B345" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G345" s="2" t="b" cm="1">
-        <f t="array" ref="G345">_xldudf_XLWINGS_READ_ERROR_CELLS(_xlfn.ANCHORARRAY(G337))</f>
+        <f t="array" ref="G345">_xldudf_XLWINGSJS_READ_ERROR_CELLS(_xlfn.ANCHORARRAY(G337))</f>
         <v>1</v>
       </c>
     </row>
@@ -7254,10 +7165,10 @@
         <v>1</v>
       </c>
       <c r="B347" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G347" s="2" t="b" cm="1">
-        <f t="array" ref="G347">_xldudf_XLWINGS_READ_ERROR_CELLS_STR(_xlfn.ANCHORARRAY(G337))</f>
+        <f t="array" ref="G347">_xldudf_XLWINGSJS_READ_ERROR_CELLS_STR(_xlfn.ANCHORARRAY(G337))</f>
         <v>1</v>
       </c>
     </row>
@@ -7267,16 +7178,16 @@
         <v>1</v>
       </c>
       <c r="B349" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E349" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="E349" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="F349" s="4">
         <v>44574</v>
       </c>
       <c r="G349" s="2" cm="1" vm="7">
-        <f t="array" ref="G349">_xldudf_XLWINGS_EXPLICIT_DATE_FORMAT()</f>
+        <f t="array" ref="G349">_xldudf_XLWINGSJS_EXPLICIT_DATE_FORMAT()</f>
         <v>44574</v>
       </c>
       <c r="H349" t="b">
@@ -7290,23 +7201,156 @@
         <v>1</v>
       </c>
       <c r="B351" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G351" s="2" t="b" cm="1">
-        <f t="array" ref="G351">_xldudf_XLWINGS_NAMESPACE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="array" ref="G351">_xldudf_XLWINGSJS_NAMESPACE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A353" t="b">
         <f ca="1">G353</f>
         <v>1</v>
       </c>
       <c r="B353" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="G353" t="b" cm="1">
-        <f t="array" aca="1" ref="G353" ca="1">_xldudf_XLWINGS_VOLATILE()</f>
+        <v>122</v>
+      </c>
+      <c r="G353" s="2" t="b" cm="1">
+        <f t="array" aca="1" ref="G353" ca="1">_xldudf_XLWINGSJS_VOLATILE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A355" t="b">
+        <f>AND(K355:M358)</f>
+        <v>1</v>
+      </c>
+      <c r="B355" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E355" t="s">
+        <v>110</v>
+      </c>
+      <c r="F355" t="s">
+        <v>111</v>
+      </c>
+      <c r="G355" s="2" t="str" cm="1">
+        <f t="array" ref="G355:I358">_xldudf_XLWINGSJS_VARARGS_ARG_DECORATOR(E355:F356,E355:F356,E355:F356)</f>
+        <v/>
+      </c>
+      <c r="H355" s="2" t="str">
+        <v>one</v>
+      </c>
+      <c r="I355" s="2" t="str">
+        <v>two</v>
+      </c>
+      <c r="K355" t="b">
+        <f>D355=G355</f>
+        <v>1</v>
+      </c>
+      <c r="L355" t="b">
+        <f t="shared" ref="L355:M358" si="61">E355=H355</f>
+        <v>1</v>
+      </c>
+      <c r="M355" t="b">
+        <f t="shared" si="61"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D356">
+        <v>0</v>
+      </c>
+      <c r="E356">
+        <v>1</v>
+      </c>
+      <c r="F356">
+        <v>2</v>
+      </c>
+      <c r="G356" s="2">
+        <v>0</v>
+      </c>
+      <c r="H356" s="2">
+        <v>1</v>
+      </c>
+      <c r="I356" s="2">
+        <v>2</v>
+      </c>
+      <c r="K356" t="b">
+        <f t="shared" ref="K356:K358" si="62">D356=G356</f>
+        <v>1</v>
+      </c>
+      <c r="L356" t="b">
+        <f t="shared" si="61"/>
+        <v>1</v>
+      </c>
+      <c r="M356" t="b">
+        <f t="shared" si="61"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D357">
+        <v>0</v>
+      </c>
+      <c r="E357">
+        <v>1</v>
+      </c>
+      <c r="F357">
+        <v>2</v>
+      </c>
+      <c r="G357" s="2">
+        <v>0</v>
+      </c>
+      <c r="H357" s="2">
+        <v>1</v>
+      </c>
+      <c r="I357" s="2">
+        <v>2</v>
+      </c>
+      <c r="K357" t="b">
+        <f t="shared" si="62"/>
+        <v>1</v>
+      </c>
+      <c r="L357" t="b">
+        <f t="shared" si="61"/>
+        <v>1</v>
+      </c>
+      <c r="M357" t="b">
+        <f t="shared" si="61"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D358">
+        <v>0</v>
+      </c>
+      <c r="E358">
+        <v>1</v>
+      </c>
+      <c r="F358">
+        <v>2</v>
+      </c>
+      <c r="G358" s="2">
+        <v>0</v>
+      </c>
+      <c r="H358" s="2">
+        <v>1</v>
+      </c>
+      <c r="I358" s="2">
+        <v>2</v>
+      </c>
+      <c r="K358" t="b">
+        <f t="shared" si="62"/>
+        <v>1</v>
+      </c>
+      <c r="L358" t="b">
+        <f t="shared" si="61"/>
+        <v>1</v>
+      </c>
+      <c r="M358" t="b">
+        <f t="shared" si="61"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added custom functions tests for type hints
</commit_message>
<xml_diff>
--- a/xlwingsjs/tests/udf_tests_officejs.xlsx
+++ b/xlwingsjs/tests/udf_tests_officejs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/dev/xlwings/xlwingsjs/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB61C120-ACDD-C44C-BB7D-B2A9432C88F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F41CCA-4CF8-6140-967D-54A3A4EFCE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1860" yWindow="-21100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="130">
   <si>
     <t>epected</t>
   </si>
@@ -505,6 +505,21 @@
   </si>
   <si>
     <t>varargs_arg_decorator</t>
+  </si>
+  <si>
+    <t>type_hints_arg</t>
+  </si>
+  <si>
+    <t>type_hints_arg_annotated</t>
+  </si>
+  <si>
+    <t>type_hints_ret_annotated</t>
+  </si>
+  <si>
+    <t>type_hints_ret_decorator_override</t>
+  </si>
+  <si>
+    <t>type_hints_arg_decorator_coexistence</t>
   </si>
 </sst>
 </file>
@@ -664,7 +679,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1225,6 +1247,12 @@
         <we:customFunctionIds>_xldudf_XLWINGSJS_READ_VERTICAL_NPARRAY</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_READ_WORKBOOK_CALLER</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_RETURN_PD_NAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_ANNOTATED</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DECORATOR_COEXISTENCE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_RET_ANNOTATED</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_RET_DECORATOR_OVERRIDE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_VARARGS_ARG_DECORATOR</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_VARIABLE_ARGS</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_VOLATILE</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_2DLIST</we:customFunctionIds>
@@ -1272,11 +1300,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P358"/>
+  <dimension ref="A1:P378"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G355" sqref="G355"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7354,19 +7380,285 @@
         <v>1</v>
       </c>
     </row>
+    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A360" t="b">
+        <f>G360</f>
+        <v>1</v>
+      </c>
+      <c r="B360" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="E360" t="s">
+        <v>110</v>
+      </c>
+      <c r="F360" t="s">
+        <v>111</v>
+      </c>
+      <c r="G360" s="2" t="b" cm="1">
+        <f t="array" ref="G360">_xldudf_XLWINGSJS_TYPE_HINTS_ARG(D360:F362)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D361">
+        <v>0</v>
+      </c>
+      <c r="E361">
+        <v>1</v>
+      </c>
+      <c r="F361">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D362">
+        <v>1</v>
+      </c>
+      <c r="E362">
+        <v>3</v>
+      </c>
+      <c r="F362">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A364" t="b">
+        <f>G364</f>
+        <v>1</v>
+      </c>
+      <c r="B364" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="E364" t="s">
+        <v>110</v>
+      </c>
+      <c r="F364" t="s">
+        <v>111</v>
+      </c>
+      <c r="G364" s="2" t="b" cm="1">
+        <f t="array" ref="G364">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_ANNOTATED(D364:F366)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D365">
+        <v>0</v>
+      </c>
+      <c r="E365">
+        <v>1</v>
+      </c>
+      <c r="F365">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D366">
+        <v>1</v>
+      </c>
+      <c r="E366">
+        <v>3</v>
+      </c>
+      <c r="F366">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A368" t="b">
+        <f>AND(_xlfn.ANCHORARRAY(J368))</f>
+        <v>1</v>
+      </c>
+      <c r="B368" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="E368" t="s">
+        <v>110</v>
+      </c>
+      <c r="F368" t="s">
+        <v>111</v>
+      </c>
+      <c r="G368" s="2" t="str" cm="1">
+        <f t="array" ref="G368:H370">_xldudf_XLWINGSJS_TYPE_HINTS_RET_ANNOTATED()</f>
+        <v>one</v>
+      </c>
+      <c r="H368" s="2" t="str">
+        <v>two</v>
+      </c>
+      <c r="J368" t="b" cm="1">
+        <f t="array" ref="J368:K370">_xlfn.ANCHORARRAY(G368)=E368:F370</f>
+        <v>1</v>
+      </c>
+      <c r="K368" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E369">
+        <v>1</v>
+      </c>
+      <c r="F369">
+        <v>2</v>
+      </c>
+      <c r="G369" s="2">
+        <v>1</v>
+      </c>
+      <c r="H369" s="2">
+        <v>2</v>
+      </c>
+      <c r="J369" t="b">
+        <v>1</v>
+      </c>
+      <c r="K369" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E370">
+        <v>3</v>
+      </c>
+      <c r="F370">
+        <v>4</v>
+      </c>
+      <c r="G370" s="2">
+        <v>3</v>
+      </c>
+      <c r="H370" s="2">
+        <v>4</v>
+      </c>
+      <c r="J370" t="b">
+        <v>1</v>
+      </c>
+      <c r="K370" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A372" t="b">
+        <f>AND(_xlfn.ANCHORARRAY(J372))</f>
+        <v>1</v>
+      </c>
+      <c r="B372" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="E372" t="s">
+        <v>110</v>
+      </c>
+      <c r="F372" t="s">
+        <v>111</v>
+      </c>
+      <c r="G372" s="2" t="str" cm="1">
+        <f t="array" ref="G372:H374">_xldudf_XLWINGSJS_TYPE_HINTS_RET_DECORATOR_OVERRIDE()</f>
+        <v>one</v>
+      </c>
+      <c r="H372" s="2" t="str">
+        <v>two</v>
+      </c>
+      <c r="J372" t="b" cm="1">
+        <f t="array" ref="J372:K374">_xlfn.ANCHORARRAY(G372)=E372:F374</f>
+        <v>1</v>
+      </c>
+      <c r="K372" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E373">
+        <v>1</v>
+      </c>
+      <c r="F373">
+        <v>2</v>
+      </c>
+      <c r="G373" s="2">
+        <v>1</v>
+      </c>
+      <c r="H373" s="2">
+        <v>2</v>
+      </c>
+      <c r="J373" t="b">
+        <v>1</v>
+      </c>
+      <c r="K373" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E374">
+        <v>3</v>
+      </c>
+      <c r="F374">
+        <v>4</v>
+      </c>
+      <c r="G374" s="2">
+        <v>3</v>
+      </c>
+      <c r="H374" s="2">
+        <v>4</v>
+      </c>
+      <c r="J374" t="b">
+        <v>1</v>
+      </c>
+      <c r="K374" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A376" t="b">
+        <f>G376</f>
+        <v>1</v>
+      </c>
+      <c r="B376" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E376" t="s">
+        <v>110</v>
+      </c>
+      <c r="F376" t="s">
+        <v>111</v>
+      </c>
+      <c r="G376" s="2" t="b" cm="1">
+        <f t="array" ref="G376">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DECORATOR_COEXISTENCE(D376:F378)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D377">
+        <v>0</v>
+      </c>
+      <c r="E377">
+        <v>1</v>
+      </c>
+      <c r="F377">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D378">
+        <v>1</v>
+      </c>
+      <c r="E378">
+        <v>3</v>
+      </c>
+      <c r="F378">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:A97 A99:A170 A172:A283 A285 A289:A290 A298 A302 A306 A309 A312:A313 A317 A319:A1048576">
-    <cfRule type="containsErrors" dxfId="2" priority="18">
+  <conditionalFormatting sqref="A3:A97 A99:A170 A172:A283 A285 A289:A290 A298 A302 A306 A309 A312:A313 A317 A319:A359 A379:A1048576">
+    <cfRule type="containsErrors" dxfId="3" priority="19">
       <formula>ISERROR(A3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A170 A172:A1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="A3:A170">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A172:A1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",A172)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
more type hint tests
</commit_message>
<xml_diff>
--- a/xlwingsjs/tests/udf_tests_officejs.xlsx
+++ b/xlwingsjs/tests/udf_tests_officejs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/dev/xlwings/xlwingsjs/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F41CCA-4CF8-6140-967D-54A3A4EFCE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CB7C6D-979D-6544-9794-A4693865A94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1860" yWindow="-21100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="141">
   <si>
     <t>epected</t>
   </si>
@@ -507,19 +507,52 @@
     <t>varargs_arg_decorator</t>
   </si>
   <si>
-    <t>type_hints_arg</t>
-  </si>
-  <si>
-    <t>type_hints_arg_annotated</t>
-  </si>
-  <si>
-    <t>type_hints_ret_annotated</t>
-  </si>
-  <si>
-    <t>type_hints_ret_decorator_override</t>
-  </si>
-  <si>
-    <t>type_hints_arg_decorator_coexistence</t>
+    <t>type_hints_arg_float</t>
+  </si>
+  <si>
+    <t>type_hints_arg_str</t>
+  </si>
+  <si>
+    <t>type_hints_arg_bool</t>
+  </si>
+  <si>
+    <t>type_hints_arg_int</t>
+  </si>
+  <si>
+    <t>type_hints_arg_datetime</t>
+  </si>
+  <si>
+    <t>type_hints_arg_df</t>
+  </si>
+  <si>
+    <t>type_hints_arg_df_annotated</t>
+  </si>
+  <si>
+    <t>type_hints_ret_df_annotated</t>
+  </si>
+  <si>
+    <t>type_hints_ret_df_decorator_override</t>
+  </si>
+  <si>
+    <t>type_hints_arg_df_decorator_coexistence</t>
+  </si>
+  <si>
+    <t>type_hints_arg_list</t>
+  </si>
+  <si>
+    <t>type_hints_arg_list_int</t>
+  </si>
+  <si>
+    <t>type_hints_arg_list_list_int</t>
+  </si>
+  <si>
+    <t>type_hints_arg_dict</t>
+  </si>
+  <si>
+    <t>type_hints_arg_array</t>
+  </si>
+  <si>
+    <t>type_hints_arg_ndarray</t>
   </si>
 </sst>
 </file>
@@ -529,7 +562,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -581,8 +614,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -607,6 +647,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5D9F1"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -621,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -674,6 +720,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,7 +1217,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="0" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1247,11 +1298,22 @@
         <we:customFunctionIds>_xldudf_XLWINGSJS_READ_VERTICAL_NPARRAY</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_READ_WORKBOOK_CALLER</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_RETURN_PD_NAT</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_ANNOTATED</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DECORATOR_COEXISTENCE</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_RET_ANNOTATED</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_RET_DECORATOR_OVERRIDE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_ARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_BOOL</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DATETIME</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF_ANNOTATED</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF_DECORATOR_COEXISTENCE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DICT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_FLOAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_INT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST_INT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST_LIST_INT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_NDARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_STR</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_RET_DF_ANNOTATED</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_RET_DF_DECORATOR_OVERRIDE</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_VARARGS_ARG_DECORATOR</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_VARIABLE_ARGS</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_VOLATILE</we:customFunctionIds>
@@ -1300,9 +1362,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P378"/>
+  <dimension ref="A1:P404"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7234,7 +7298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A353" t="b">
         <f ca="1">G353</f>
         <v>1</v>
@@ -7247,7 +7311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A355" t="b">
         <f>AND(K355:M358)</f>
         <v>1</v>
@@ -7284,7 +7348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D356">
         <v>0</v>
       </c>
@@ -7316,7 +7380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D357">
         <v>0</v>
       </c>
@@ -7348,7 +7412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D358">
         <v>0</v>
       </c>
@@ -7380,269 +7444,502 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A360" t="b">
-        <f>G360</f>
-        <v>1</v>
-      </c>
-      <c r="B360" s="23" t="s">
+    <row r="361" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A361" t="b">
+        <f>G361</f>
+        <v>1</v>
+      </c>
+      <c r="B361" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C361" s="27"/>
+      <c r="D361" s="27"/>
+      <c r="E361" s="27"/>
+      <c r="F361" s="27">
+        <v>2</v>
+      </c>
+      <c r="G361" s="28" t="b" cm="1">
+        <f t="array" ref="G361">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_INT(F361)</f>
+        <v>1</v>
+      </c>
+      <c r="H361" s="27"/>
+      <c r="I361" s="27"/>
+      <c r="J361" s="27"/>
+      <c r="K361" s="27"/>
+      <c r="L361" s="27"/>
+      <c r="M361" s="27"/>
+      <c r="N361" s="27"/>
+      <c r="O361" s="27"/>
+      <c r="P361" s="27"/>
+    </row>
+    <row r="363" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A363" t="b">
+        <f>G363</f>
+        <v>1</v>
+      </c>
+      <c r="B363" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="E360" t="s">
+      <c r="F363">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G363" s="2" t="b" cm="1">
+        <f t="array" ref="G363">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_FLOAT(F363)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A365" t="b">
+        <f>G365</f>
+        <v>1</v>
+      </c>
+      <c r="B365" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F365" t="s">
+        <v>2</v>
+      </c>
+      <c r="G365" s="2" t="b" cm="1">
+        <f t="array" ref="G365">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_STR(F365)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A367" t="b">
+        <f>G367</f>
+        <v>1</v>
+      </c>
+      <c r="B367" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F367" t="b">
+        <v>1</v>
+      </c>
+      <c r="G367" s="2" t="b" cm="1">
+        <f t="array" ref="G367">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_BOOL(F367)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B368" s="23"/>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A369" t="b">
+        <f>G369</f>
+        <v>1</v>
+      </c>
+      <c r="B369" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="F369" s="4">
+        <v>44185</v>
+      </c>
+      <c r="G369" s="2" t="b" cm="1">
+        <f t="array" ref="G369">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DATETIME(F369)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A371" t="b">
+        <f>G371</f>
+        <v>1</v>
+      </c>
+      <c r="B371" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E371">
+        <v>1</v>
+      </c>
+      <c r="F371">
+        <v>2</v>
+      </c>
+      <c r="G371" s="2" t="b" cm="1">
+        <f t="array" ref="G371">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST(E371:F371)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A373" t="b">
+        <f>G373</f>
+        <v>1</v>
+      </c>
+      <c r="B373" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E373">
+        <v>1</v>
+      </c>
+      <c r="F373">
+        <v>2</v>
+      </c>
+      <c r="G373" s="2" t="b" cm="1">
+        <f t="array" ref="G373">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST_INT(E373:F373)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A375" t="b">
+        <f>G375</f>
+        <v>1</v>
+      </c>
+      <c r="B375" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E375">
+        <v>1</v>
+      </c>
+      <c r="F375">
+        <v>2</v>
+      </c>
+      <c r="G375" s="2" t="b" cm="1">
+        <f t="array" ref="G375">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST_LIST_INT(E375:F376)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E376">
+        <v>3</v>
+      </c>
+      <c r="F376">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A378" t="b">
+        <f>G378</f>
+        <v>1</v>
+      </c>
+      <c r="B378" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E378" t="s">
+        <v>50</v>
+      </c>
+      <c r="F378">
+        <v>1</v>
+      </c>
+      <c r="G378" s="2" t="b" cm="1">
+        <f t="array" ref="G378">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DICT(E378:F378)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A380" t="b">
+        <f>G380</f>
+        <v>1</v>
+      </c>
+      <c r="B380" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E380">
+        <v>1</v>
+      </c>
+      <c r="F380">
+        <v>2</v>
+      </c>
+      <c r="G380" s="2" t="b" cm="1">
+        <f t="array" ref="G380">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_ARRAY(E380:F381)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E381">
+        <v>3</v>
+      </c>
+      <c r="F381">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A383" t="b">
+        <f>G383</f>
+        <v>1</v>
+      </c>
+      <c r="B383" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E383">
+        <v>1</v>
+      </c>
+      <c r="F383">
+        <v>2</v>
+      </c>
+      <c r="G383" s="2" t="b" cm="1">
+        <f t="array" ref="G383">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_NDARRAY(E383:F384)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E384">
+        <v>3</v>
+      </c>
+      <c r="F384">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A386" t="b">
+        <f>G386</f>
+        <v>1</v>
+      </c>
+      <c r="B386" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E386" t="s">
         <v>110</v>
       </c>
-      <c r="F360" t="s">
+      <c r="F386" t="s">
         <v>111</v>
       </c>
-      <c r="G360" s="2" t="b" cm="1">
-        <f t="array" ref="G360">_xldudf_XLWINGSJS_TYPE_HINTS_ARG(D360:F362)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D361">
+      <c r="G386" s="2" t="b" cm="1">
+        <f t="array" ref="G386">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF(D386:F388)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D387">
         <v>0</v>
       </c>
-      <c r="E361">
-        <v>1</v>
-      </c>
-      <c r="F361">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D362">
-        <v>1</v>
-      </c>
-      <c r="E362">
+      <c r="E387">
+        <v>1</v>
+      </c>
+      <c r="F387">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D388">
+        <v>1</v>
+      </c>
+      <c r="E388">
         <v>3</v>
       </c>
-      <c r="F362">
+      <c r="F388">
         <v>4</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A364" t="b">
-        <f>G364</f>
-        <v>1</v>
-      </c>
-      <c r="B364" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="E364" t="s">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A390" t="b">
+        <f>G390</f>
+        <v>1</v>
+      </c>
+      <c r="B390" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E390" t="s">
         <v>110</v>
       </c>
-      <c r="F364" t="s">
+      <c r="F390" t="s">
         <v>111</v>
       </c>
-      <c r="G364" s="2" t="b" cm="1">
-        <f t="array" ref="G364">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_ANNOTATED(D364:F366)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D365">
+      <c r="G390" s="2" t="b" cm="1">
+        <f t="array" ref="G390">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF_ANNOTATED(D390:F392)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D391">
         <v>0</v>
       </c>
-      <c r="E365">
-        <v>1</v>
-      </c>
-      <c r="F365">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D366">
-        <v>1</v>
-      </c>
-      <c r="E366">
+      <c r="E391">
+        <v>1</v>
+      </c>
+      <c r="F391">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D392">
+        <v>1</v>
+      </c>
+      <c r="E392">
         <v>3</v>
       </c>
-      <c r="F366">
+      <c r="F392">
         <v>4</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A368" t="b">
-        <f>AND(_xlfn.ANCHORARRAY(J368))</f>
-        <v>1</v>
-      </c>
-      <c r="B368" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="E368" t="s">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A394" t="b">
+        <f>AND(_xlfn.ANCHORARRAY(J394))</f>
+        <v>1</v>
+      </c>
+      <c r="B394" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E394" t="s">
         <v>110</v>
       </c>
-      <c r="F368" t="s">
+      <c r="F394" t="s">
         <v>111</v>
       </c>
-      <c r="G368" s="2" t="str" cm="1">
-        <f t="array" ref="G368:H370">_xldudf_XLWINGSJS_TYPE_HINTS_RET_ANNOTATED()</f>
+      <c r="G394" s="2" t="str" cm="1">
+        <f t="array" ref="G394:H396">_xldudf_XLWINGSJS_TYPE_HINTS_RET_DF_ANNOTATED()</f>
         <v>one</v>
       </c>
-      <c r="H368" s="2" t="str">
+      <c r="H394" s="2" t="str">
         <v>two</v>
       </c>
-      <c r="J368" t="b" cm="1">
-        <f t="array" ref="J368:K370">_xlfn.ANCHORARRAY(G368)=E368:F370</f>
-        <v>1</v>
-      </c>
-      <c r="K368" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E369">
-        <v>1</v>
-      </c>
-      <c r="F369">
-        <v>2</v>
-      </c>
-      <c r="G369" s="2">
-        <v>1</v>
-      </c>
-      <c r="H369" s="2">
-        <v>2</v>
-      </c>
-      <c r="J369" t="b">
-        <v>1</v>
-      </c>
-      <c r="K369" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E370">
+      <c r="J394" t="b" cm="1">
+        <f t="array" ref="J394:K396">_xlfn.ANCHORARRAY(G394)=E394:F396</f>
+        <v>1</v>
+      </c>
+      <c r="K394" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E395">
+        <v>1</v>
+      </c>
+      <c r="F395">
+        <v>2</v>
+      </c>
+      <c r="G395" s="2">
+        <v>1</v>
+      </c>
+      <c r="H395" s="2">
+        <v>2</v>
+      </c>
+      <c r="J395" t="b">
+        <v>1</v>
+      </c>
+      <c r="K395" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E396">
         <v>3</v>
       </c>
-      <c r="F370">
+      <c r="F396">
         <v>4</v>
       </c>
-      <c r="G370" s="2">
+      <c r="G396" s="2">
         <v>3</v>
       </c>
-      <c r="H370" s="2">
+      <c r="H396" s="2">
         <v>4</v>
       </c>
-      <c r="J370" t="b">
-        <v>1</v>
-      </c>
-      <c r="K370" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A372" t="b">
-        <f>AND(_xlfn.ANCHORARRAY(J372))</f>
-        <v>1</v>
-      </c>
-      <c r="B372" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E372" t="s">
+      <c r="J396" t="b">
+        <v>1</v>
+      </c>
+      <c r="K396" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A398" t="b">
+        <f>AND(_xlfn.ANCHORARRAY(J398))</f>
+        <v>1</v>
+      </c>
+      <c r="B398" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="E398" t="s">
         <v>110</v>
       </c>
-      <c r="F372" t="s">
+      <c r="F398" t="s">
         <v>111</v>
       </c>
-      <c r="G372" s="2" t="str" cm="1">
-        <f t="array" ref="G372:H374">_xldudf_XLWINGSJS_TYPE_HINTS_RET_DECORATOR_OVERRIDE()</f>
+      <c r="G398" s="2" t="str" cm="1">
+        <f t="array" ref="G398:H400">_xldudf_XLWINGSJS_TYPE_HINTS_RET_DF_DECORATOR_OVERRIDE()</f>
         <v>one</v>
       </c>
-      <c r="H372" s="2" t="str">
+      <c r="H398" s="2" t="str">
         <v>two</v>
       </c>
-      <c r="J372" t="b" cm="1">
-        <f t="array" ref="J372:K374">_xlfn.ANCHORARRAY(G372)=E372:F374</f>
-        <v>1</v>
-      </c>
-      <c r="K372" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E373">
-        <v>1</v>
-      </c>
-      <c r="F373">
-        <v>2</v>
-      </c>
-      <c r="G373" s="2">
-        <v>1</v>
-      </c>
-      <c r="H373" s="2">
-        <v>2</v>
-      </c>
-      <c r="J373" t="b">
-        <v>1</v>
-      </c>
-      <c r="K373" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E374">
+      <c r="J398" t="b" cm="1">
+        <f t="array" ref="J398:K400">_xlfn.ANCHORARRAY(G398)=E398:F400</f>
+        <v>1</v>
+      </c>
+      <c r="K398" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E399">
+        <v>1</v>
+      </c>
+      <c r="F399">
+        <v>2</v>
+      </c>
+      <c r="G399" s="2">
+        <v>1</v>
+      </c>
+      <c r="H399" s="2">
+        <v>2</v>
+      </c>
+      <c r="J399" t="b">
+        <v>1</v>
+      </c>
+      <c r="K399" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E400">
         <v>3</v>
       </c>
-      <c r="F374">
+      <c r="F400">
         <v>4</v>
       </c>
-      <c r="G374" s="2">
+      <c r="G400" s="2">
         <v>3</v>
       </c>
-      <c r="H374" s="2">
+      <c r="H400" s="2">
         <v>4</v>
       </c>
-      <c r="J374" t="b">
-        <v>1</v>
-      </c>
-      <c r="K374" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A376" t="b">
-        <f>G376</f>
-        <v>1</v>
-      </c>
-      <c r="B376" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="E376" t="s">
+      <c r="J400" t="b">
+        <v>1</v>
+      </c>
+      <c r="K400" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A402" t="b">
+        <f>G402</f>
+        <v>1</v>
+      </c>
+      <c r="B402" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E402" t="s">
         <v>110</v>
       </c>
-      <c r="F376" t="s">
+      <c r="F402" t="s">
         <v>111</v>
       </c>
-      <c r="G376" s="2" t="b" cm="1">
-        <f t="array" ref="G376">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DECORATOR_COEXISTENCE(D376:F378)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D377">
+      <c r="G402" s="2" t="b" cm="1">
+        <f t="array" ref="G402">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF_DECORATOR_COEXISTENCE(D402:F404)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D403">
         <v>0</v>
       </c>
-      <c r="E377">
-        <v>1</v>
-      </c>
-      <c r="F377">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D378">
-        <v>1</v>
-      </c>
-      <c r="E378">
+      <c r="E403">
+        <v>1</v>
+      </c>
+      <c r="F403">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D404">
+        <v>1</v>
+      </c>
+      <c r="E404">
         <v>3</v>
       </c>
-      <c r="F378">
+      <c r="F404">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:A97 A99:A170 A172:A283 A285 A289:A290 A298 A302 A306 A309 A312:A313 A317 A319:A359 A379:A1048576">
+  <conditionalFormatting sqref="A3:A97 A99:A170 A172:A283 A285 A289:A290 A298 A302 A306 A309 A312:A313 A317 A319:A360 A362 A366 A370 A405:A1048576 A372 A374 A376:A377 A379 A381:A382 A384:A385">
     <cfRule type="containsErrors" dxfId="3" priority="19">
       <formula>ISERROR(A3)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Type hint converters (requires Python 3.9+) (#2494)
* accept type hints in custom functions instead of decorator convert args

* Add support for typing.Annotations

* Add type hint support for classic UDFs

* added udf test for type hints

* added custom functions tests for type hints

* make basic type hints use the default converter and make the default converter accessible via "default" name

* more type hint tests

* docs
</commit_message>
<xml_diff>
--- a/xlwingsjs/tests/udf_tests_officejs.xlsx
+++ b/xlwingsjs/tests/udf_tests_officejs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/dev/xlwings/xlwingsjs/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB61C120-ACDD-C44C-BB7D-B2A9432C88F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CB7C6D-979D-6544-9794-A4693865A94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1860" yWindow="-21100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="141">
   <si>
     <t>epected</t>
   </si>
@@ -505,6 +505,54 @@
   </si>
   <si>
     <t>varargs_arg_decorator</t>
+  </si>
+  <si>
+    <t>type_hints_arg_float</t>
+  </si>
+  <si>
+    <t>type_hints_arg_str</t>
+  </si>
+  <si>
+    <t>type_hints_arg_bool</t>
+  </si>
+  <si>
+    <t>type_hints_arg_int</t>
+  </si>
+  <si>
+    <t>type_hints_arg_datetime</t>
+  </si>
+  <si>
+    <t>type_hints_arg_df</t>
+  </si>
+  <si>
+    <t>type_hints_arg_df_annotated</t>
+  </si>
+  <si>
+    <t>type_hints_ret_df_annotated</t>
+  </si>
+  <si>
+    <t>type_hints_ret_df_decorator_override</t>
+  </si>
+  <si>
+    <t>type_hints_arg_df_decorator_coexistence</t>
+  </si>
+  <si>
+    <t>type_hints_arg_list</t>
+  </si>
+  <si>
+    <t>type_hints_arg_list_int</t>
+  </si>
+  <si>
+    <t>type_hints_arg_list_list_int</t>
+  </si>
+  <si>
+    <t>type_hints_arg_dict</t>
+  </si>
+  <si>
+    <t>type_hints_arg_array</t>
+  </si>
+  <si>
+    <t>type_hints_arg_ndarray</t>
   </si>
 </sst>
 </file>
@@ -514,7 +562,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -566,8 +614,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -592,6 +647,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5D9F1"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -606,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -659,12 +720,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1144,7 +1217,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="0" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1225,6 +1298,23 @@
         <we:customFunctionIds>_xldudf_XLWINGSJS_READ_VERTICAL_NPARRAY</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_READ_WORKBOOK_CALLER</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_RETURN_PD_NAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_ARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_BOOL</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DATETIME</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF_ANNOTATED</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF_DECORATOR_COEXISTENCE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DICT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_FLOAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_INT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST_INT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST_LIST_INT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_NDARRAY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_ARG_STR</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_RET_DF_ANNOTATED</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_TYPE_HINTS_RET_DF_DECORATOR_OVERRIDE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_XLWINGSJS_VARARGS_ARG_DECORATOR</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_VARIABLE_ARGS</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_VOLATILE</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_XLWINGSJS_WRITE_2DLIST</we:customFunctionIds>
@@ -1272,10 +1362,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P358"/>
+  <dimension ref="A1:P404"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G355" sqref="G355"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7208,7 +7298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A353" t="b">
         <f ca="1">G353</f>
         <v>1</v>
@@ -7221,7 +7311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A355" t="b">
         <f>AND(K355:M358)</f>
         <v>1</v>
@@ -7258,7 +7348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D356">
         <v>0</v>
       </c>
@@ -7290,7 +7380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D357">
         <v>0</v>
       </c>
@@ -7322,7 +7412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D358">
         <v>0</v>
       </c>
@@ -7354,19 +7444,518 @@
         <v>1</v>
       </c>
     </row>
+    <row r="361" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A361" t="b">
+        <f>G361</f>
+        <v>1</v>
+      </c>
+      <c r="B361" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C361" s="27"/>
+      <c r="D361" s="27"/>
+      <c r="E361" s="27"/>
+      <c r="F361" s="27">
+        <v>2</v>
+      </c>
+      <c r="G361" s="28" t="b" cm="1">
+        <f t="array" ref="G361">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_INT(F361)</f>
+        <v>1</v>
+      </c>
+      <c r="H361" s="27"/>
+      <c r="I361" s="27"/>
+      <c r="J361" s="27"/>
+      <c r="K361" s="27"/>
+      <c r="L361" s="27"/>
+      <c r="M361" s="27"/>
+      <c r="N361" s="27"/>
+      <c r="O361" s="27"/>
+      <c r="P361" s="27"/>
+    </row>
+    <row r="363" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A363" t="b">
+        <f>G363</f>
+        <v>1</v>
+      </c>
+      <c r="B363" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="F363">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G363" s="2" t="b" cm="1">
+        <f t="array" ref="G363">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_FLOAT(F363)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A365" t="b">
+        <f>G365</f>
+        <v>1</v>
+      </c>
+      <c r="B365" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F365" t="s">
+        <v>2</v>
+      </c>
+      <c r="G365" s="2" t="b" cm="1">
+        <f t="array" ref="G365">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_STR(F365)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A367" t="b">
+        <f>G367</f>
+        <v>1</v>
+      </c>
+      <c r="B367" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F367" t="b">
+        <v>1</v>
+      </c>
+      <c r="G367" s="2" t="b" cm="1">
+        <f t="array" ref="G367">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_BOOL(F367)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B368" s="23"/>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A369" t="b">
+        <f>G369</f>
+        <v>1</v>
+      </c>
+      <c r="B369" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="F369" s="4">
+        <v>44185</v>
+      </c>
+      <c r="G369" s="2" t="b" cm="1">
+        <f t="array" ref="G369">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DATETIME(F369)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A371" t="b">
+        <f>G371</f>
+        <v>1</v>
+      </c>
+      <c r="B371" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E371">
+        <v>1</v>
+      </c>
+      <c r="F371">
+        <v>2</v>
+      </c>
+      <c r="G371" s="2" t="b" cm="1">
+        <f t="array" ref="G371">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST(E371:F371)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A373" t="b">
+        <f>G373</f>
+        <v>1</v>
+      </c>
+      <c r="B373" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E373">
+        <v>1</v>
+      </c>
+      <c r="F373">
+        <v>2</v>
+      </c>
+      <c r="G373" s="2" t="b" cm="1">
+        <f t="array" ref="G373">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST_INT(E373:F373)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A375" t="b">
+        <f>G375</f>
+        <v>1</v>
+      </c>
+      <c r="B375" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E375">
+        <v>1</v>
+      </c>
+      <c r="F375">
+        <v>2</v>
+      </c>
+      <c r="G375" s="2" t="b" cm="1">
+        <f t="array" ref="G375">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_LIST_LIST_INT(E375:F376)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E376">
+        <v>3</v>
+      </c>
+      <c r="F376">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A378" t="b">
+        <f>G378</f>
+        <v>1</v>
+      </c>
+      <c r="B378" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E378" t="s">
+        <v>50</v>
+      </c>
+      <c r="F378">
+        <v>1</v>
+      </c>
+      <c r="G378" s="2" t="b" cm="1">
+        <f t="array" ref="G378">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DICT(E378:F378)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A380" t="b">
+        <f>G380</f>
+        <v>1</v>
+      </c>
+      <c r="B380" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E380">
+        <v>1</v>
+      </c>
+      <c r="F380">
+        <v>2</v>
+      </c>
+      <c r="G380" s="2" t="b" cm="1">
+        <f t="array" ref="G380">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_ARRAY(E380:F381)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E381">
+        <v>3</v>
+      </c>
+      <c r="F381">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A383" t="b">
+        <f>G383</f>
+        <v>1</v>
+      </c>
+      <c r="B383" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E383">
+        <v>1</v>
+      </c>
+      <c r="F383">
+        <v>2</v>
+      </c>
+      <c r="G383" s="2" t="b" cm="1">
+        <f t="array" ref="G383">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_NDARRAY(E383:F384)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E384">
+        <v>3</v>
+      </c>
+      <c r="F384">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A386" t="b">
+        <f>G386</f>
+        <v>1</v>
+      </c>
+      <c r="B386" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E386" t="s">
+        <v>110</v>
+      </c>
+      <c r="F386" t="s">
+        <v>111</v>
+      </c>
+      <c r="G386" s="2" t="b" cm="1">
+        <f t="array" ref="G386">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF(D386:F388)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D387">
+        <v>0</v>
+      </c>
+      <c r="E387">
+        <v>1</v>
+      </c>
+      <c r="F387">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D388">
+        <v>1</v>
+      </c>
+      <c r="E388">
+        <v>3</v>
+      </c>
+      <c r="F388">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="390" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A390" t="b">
+        <f>G390</f>
+        <v>1</v>
+      </c>
+      <c r="B390" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E390" t="s">
+        <v>110</v>
+      </c>
+      <c r="F390" t="s">
+        <v>111</v>
+      </c>
+      <c r="G390" s="2" t="b" cm="1">
+        <f t="array" ref="G390">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF_ANNOTATED(D390:F392)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D391">
+        <v>0</v>
+      </c>
+      <c r="E391">
+        <v>1</v>
+      </c>
+      <c r="F391">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D392">
+        <v>1</v>
+      </c>
+      <c r="E392">
+        <v>3</v>
+      </c>
+      <c r="F392">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A394" t="b">
+        <f>AND(_xlfn.ANCHORARRAY(J394))</f>
+        <v>1</v>
+      </c>
+      <c r="B394" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E394" t="s">
+        <v>110</v>
+      </c>
+      <c r="F394" t="s">
+        <v>111</v>
+      </c>
+      <c r="G394" s="2" t="str" cm="1">
+        <f t="array" ref="G394:H396">_xldudf_XLWINGSJS_TYPE_HINTS_RET_DF_ANNOTATED()</f>
+        <v>one</v>
+      </c>
+      <c r="H394" s="2" t="str">
+        <v>two</v>
+      </c>
+      <c r="J394" t="b" cm="1">
+        <f t="array" ref="J394:K396">_xlfn.ANCHORARRAY(G394)=E394:F396</f>
+        <v>1</v>
+      </c>
+      <c r="K394" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E395">
+        <v>1</v>
+      </c>
+      <c r="F395">
+        <v>2</v>
+      </c>
+      <c r="G395" s="2">
+        <v>1</v>
+      </c>
+      <c r="H395" s="2">
+        <v>2</v>
+      </c>
+      <c r="J395" t="b">
+        <v>1</v>
+      </c>
+      <c r="K395" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E396">
+        <v>3</v>
+      </c>
+      <c r="F396">
+        <v>4</v>
+      </c>
+      <c r="G396" s="2">
+        <v>3</v>
+      </c>
+      <c r="H396" s="2">
+        <v>4</v>
+      </c>
+      <c r="J396" t="b">
+        <v>1</v>
+      </c>
+      <c r="K396" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A398" t="b">
+        <f>AND(_xlfn.ANCHORARRAY(J398))</f>
+        <v>1</v>
+      </c>
+      <c r="B398" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="E398" t="s">
+        <v>110</v>
+      </c>
+      <c r="F398" t="s">
+        <v>111</v>
+      </c>
+      <c r="G398" s="2" t="str" cm="1">
+        <f t="array" ref="G398:H400">_xldudf_XLWINGSJS_TYPE_HINTS_RET_DF_DECORATOR_OVERRIDE()</f>
+        <v>one</v>
+      </c>
+      <c r="H398" s="2" t="str">
+        <v>two</v>
+      </c>
+      <c r="J398" t="b" cm="1">
+        <f t="array" ref="J398:K400">_xlfn.ANCHORARRAY(G398)=E398:F400</f>
+        <v>1</v>
+      </c>
+      <c r="K398" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E399">
+        <v>1</v>
+      </c>
+      <c r="F399">
+        <v>2</v>
+      </c>
+      <c r="G399" s="2">
+        <v>1</v>
+      </c>
+      <c r="H399" s="2">
+        <v>2</v>
+      </c>
+      <c r="J399" t="b">
+        <v>1</v>
+      </c>
+      <c r="K399" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E400">
+        <v>3</v>
+      </c>
+      <c r="F400">
+        <v>4</v>
+      </c>
+      <c r="G400" s="2">
+        <v>3</v>
+      </c>
+      <c r="H400" s="2">
+        <v>4</v>
+      </c>
+      <c r="J400" t="b">
+        <v>1</v>
+      </c>
+      <c r="K400" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A402" t="b">
+        <f>G402</f>
+        <v>1</v>
+      </c>
+      <c r="B402" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E402" t="s">
+        <v>110</v>
+      </c>
+      <c r="F402" t="s">
+        <v>111</v>
+      </c>
+      <c r="G402" s="2" t="b" cm="1">
+        <f t="array" ref="G402">_xldudf_XLWINGSJS_TYPE_HINTS_ARG_DF_DECORATOR_COEXISTENCE(D402:F404)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D403">
+        <v>0</v>
+      </c>
+      <c r="E403">
+        <v>1</v>
+      </c>
+      <c r="F403">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D404">
+        <v>1</v>
+      </c>
+      <c r="E404">
+        <v>3</v>
+      </c>
+      <c r="F404">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:A97 A99:A170 A172:A283 A285 A289:A290 A298 A302 A306 A309 A312:A313 A317 A319:A1048576">
-    <cfRule type="containsErrors" dxfId="2" priority="18">
+  <conditionalFormatting sqref="A3:A97 A99:A170 A172:A283 A285 A289:A290 A298 A302 A306 A309 A312:A313 A317 A319:A360 A362 A366 A370 A405:A1048576 A372 A374 A376:A377 A379 A381:A382 A384:A385">
+    <cfRule type="containsErrors" dxfId="3" priority="19">
       <formula>ISERROR(A3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A170 A172:A1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="A3:A170">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A172:A1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",A172)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>